<commit_message>
customer overview feature file added. made few changes to cross sell page tests.
</commit_message>
<xml_diff>
--- a/testData/qa/Cross_sell.xlsx
+++ b/testData/qa/Cross_sell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naga.kumar\customerAi\testData\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF313305-507B-45B5-B361-673CCA23A78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9A6A15-22C6-4033-8E37-B9C2C7F89A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross_sell_Filter" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>DataRowNum</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Within 90 days</t>
+  </si>
+  <si>
+    <t>Selected Drivers</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Driver 1,Driver 2,Driver 3,Driver 4,Driver 5</t>
   </si>
 </sst>
 </file>
@@ -529,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE05FA26-6CCD-497E-81B2-6E2510738995}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,12 +575,14 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="H2" s="5"/>
     </row>
@@ -579,14 +590,12 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -597,10 +606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D519C6-B5E4-4FAF-A519-D5C875BF9495}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -608,11 +617,12 @@
     <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" customWidth="1"/>
+    <col min="5" max="5" width="35.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -623,13 +633,16 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -640,13 +653,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -657,30 +673,36 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -691,13 +713,16 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -708,30 +733,37 @@
         <v>26</v>
       </c>
       <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DB Validation added for drivers
</commit_message>
<xml_diff>
--- a/testData/qa/Cross_sell.xlsx
+++ b/testData/qa/Cross_sell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naga.kumar\customerAi\testData\qa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9A6A15-22C6-4033-8E37-B9C2C7F89A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EDE6EC-DB74-4D63-B9E6-102E00106E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
+    <workbookView xWindow="-40" yWindow="-40" windowWidth="19280" windowHeight="10280" xr2:uid="{EE76EA1F-E72F-46B2-BEA2-9E761BC260D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross_sell_Filter" sheetId="4" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Date Range</t>
   </si>
   <si>
-    <t>Credit Cards: Silver, Gold, Platinum &amp; Millennium</t>
-  </si>
-  <si>
     <t>Within 180 days</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Driver 1,Driver 2,Driver 3,Driver 4,Driver 5</t>
+  </si>
+  <si>
+    <t>Credit Cards</t>
   </si>
 </sst>
 </file>
@@ -538,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE05FA26-6CCD-497E-81B2-6E2510738995}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -576,13 +576,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="H2" s="5"/>
     </row>
@@ -592,10 +592,10 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -608,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D519C6-B5E4-4FAF-A519-D5C875BF9495}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -627,19 +627,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -647,19 +647,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -667,19 +667,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -687,19 +687,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -707,19 +707,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -727,19 +727,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -747,19 +747,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>